<commit_message>
verificación 06-13 y 06-01
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion01/Escaleta CN_06_01_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion01/Escaleta CN_06_01_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\German\Documents\Aulaplaneta All\Trabajos de autor\4 Sexto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mpgarcia\Desktop\CienciasNaturales\fuentes\contenidos\grado06\guion01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -707,10 +707,10 @@
     <t>Competencia</t>
   </si>
   <si>
-    <t>Actividad colaborativa que guía el trabajo colaborativo sobre el experimento de Pasteur con la utilización de materiales de fácil consecución</t>
-  </si>
-  <si>
     <t>Competencias: el experimento de Pasteur</t>
+  </si>
+  <si>
+    <t>Actividad que guía el trabajo colaborativo sobre el experimento de Pasteur</t>
   </si>
 </sst>
 </file>
@@ -1009,13 +1009,35 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1041,28 +1063,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3331,7 +3331,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
@@ -3362,94 +3362,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="J1" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="31" t="s">
+      <c r="K1" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="L1" s="30" t="s">
+      <c r="L1" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="33" t="s">
+      <c r="M1" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="34"/>
-      <c r="O1" s="27" t="s">
+      <c r="N1" s="42"/>
+      <c r="O1" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="P1" s="36" t="s">
+      <c r="P1" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="Q1" s="37" t="s">
+      <c r="Q1" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="R1" s="39" t="s">
+      <c r="R1" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="S1" s="37" t="s">
+      <c r="S1" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="T1" s="38" t="s">
+      <c r="T1" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="U1" s="37" t="s">
+      <c r="U1" s="31" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="30"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="38"/>
       <c r="M2" s="7" t="s">
         <v>92</v>
       </c>
       <c r="N2" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="38"/>
-      <c r="U2" s="37"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="31"/>
     </row>
     <row r="3" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
@@ -4771,7 +4771,7 @@
       <c r="N28" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="O28" s="40"/>
+      <c r="O28" s="25"/>
       <c r="P28" s="8" t="s">
         <v>20</v>
       </c>
@@ -4832,7 +4832,7 @@
       <c r="N29" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="O29" s="40"/>
+      <c r="O29" s="25"/>
       <c r="P29" s="8" t="s">
         <v>19</v>
       </c>
@@ -4891,7 +4891,7 @@
       <c r="N30" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="O30" s="40"/>
+      <c r="O30" s="25"/>
       <c r="P30" s="8" t="s">
         <v>19</v>
       </c>
@@ -4926,17 +4926,17 @@
       </c>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
-      <c r="G31" s="40" t="s">
+      <c r="G31" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="H31" s="26">
+        <v>21</v>
+      </c>
+      <c r="I31" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="J31" s="28" t="s">
         <v>228</v>
-      </c>
-      <c r="H31" s="41">
-        <v>21</v>
-      </c>
-      <c r="I31" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="J31" s="43" t="s">
-        <v>227</v>
       </c>
       <c r="K31" s="8" t="s">
         <v>20</v>
@@ -4948,7 +4948,7 @@
         <v>66</v>
       </c>
       <c r="N31" s="8"/>
-      <c r="O31" s="40" t="s">
+      <c r="O31" s="25" t="s">
         <v>226</v>
       </c>
       <c r="P31" s="8" t="s">
@@ -5007,7 +5007,7 @@
       <c r="N32" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="O32" s="40"/>
+      <c r="O32" s="25"/>
       <c r="P32" s="8" t="s">
         <v>19</v>
       </c>
@@ -5042,16 +5042,16 @@
       </c>
       <c r="E33" s="9"/>
       <c r="F33" s="9"/>
-      <c r="G33" s="40" t="s">
+      <c r="G33" s="25" t="s">
         <v>224</v>
       </c>
-      <c r="H33" s="41">
+      <c r="H33" s="26">
         <v>23</v>
       </c>
-      <c r="I33" s="41" t="s">
+      <c r="I33" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="J33" s="43" t="s">
+      <c r="J33" s="28" t="s">
         <v>225</v>
       </c>
       <c r="K33" s="8" t="s">
@@ -5064,7 +5064,7 @@
         <v>65</v>
       </c>
       <c r="N33" s="8"/>
-      <c r="O33" s="40" t="s">
+      <c r="O33" s="25" t="s">
         <v>226</v>
       </c>
       <c r="P33" s="8" t="s">
@@ -5119,7 +5119,7 @@
       <c r="L34" s="8"/>
       <c r="M34" s="8"/>
       <c r="N34" s="8"/>
-      <c r="O34" s="40"/>
+      <c r="O34" s="25"/>
       <c r="P34" s="8"/>
       <c r="Q34" s="10"/>
       <c r="R34" s="10"/>
@@ -5164,7 +5164,7 @@
       <c r="N35" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="O35" s="40"/>
+      <c r="O35" s="25"/>
       <c r="P35" s="17" t="s">
         <v>19</v>
       </c>
@@ -5217,7 +5217,7 @@
       <c r="N36" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="O36" s="40"/>
+      <c r="O36" s="25"/>
       <c r="P36" s="8" t="s">
         <v>19</v>
       </c>
@@ -5427,12 +5427,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -5447,6 +5441,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I8 I23 I6 I18:I20 I15:I16 P6 P8 P10 P15:P16 P19:P20 P23 P34">

</xml_diff>